<commit_message>
refactor, meet initial requirements
</commit_message>
<xml_diff>
--- a/output/2016-10.xlsx
+++ b/output/2016-10.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="PI hours" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="dept hours" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="PI hours" sheetId="1" r:id="rId1"/>
+    <sheet name="dept hours" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>name</t>
   </si>
@@ -23,22 +23,25 @@
     <t>hours</t>
   </si>
   <si>
+    <t>percentage</t>
+  </si>
+  <si>
     <t>dept</t>
   </si>
   <si>
     <t>Naira Hovakimyan</t>
   </si>
   <si>
+    <t>Girish Chowdhary</t>
+  </si>
+  <si>
+    <t>Seth Hutchinson</t>
+  </si>
+  <si>
     <t>['ME', 'AE', 'CSL']</t>
   </si>
   <si>
-    <t>Girish Chowdhary</t>
-  </si>
-  <si>
     <t>['ABE', 'CSL']</t>
-  </si>
-  <si>
-    <t>Seth Hutchinson</t>
   </si>
   <si>
     <t>['ECE', 'CSL']</t>
@@ -63,22 +66,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -93,26 +100,35 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -400,20 +416,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -423,132 +433,156 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="1" t="n">
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C2">
         <v>39</v>
       </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="1" t="n">
+      <c r="D2">
+        <v>70.90909090909091</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3">
+        <v>14.54545454545454</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="n">
+      <c r="C4">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
-        <v>8</v>
+      <c r="D4">
+        <v>14.54545454545454</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="n">
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="n">
+        <v>10</v>
+      </c>
+      <c r="C2">
         <v>55</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="n">
+      <c r="D2">
+        <v>36.91275167785235</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="n">
+        <v>11</v>
+      </c>
+      <c r="C3">
         <v>39</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1" t="n">
+      <c r="D3">
+        <v>26.1744966442953</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="n">
+        <v>12</v>
+      </c>
+      <c r="C4">
         <v>39</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1" t="n">
+      <c r="D4">
+        <v>26.1744966442953</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="n">
+        <v>13</v>
+      </c>
+      <c r="C5">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1" t="n">
+      <c r="D5">
+        <v>5.369127516778524</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="n">
+        <v>14</v>
+      </c>
+      <c r="C6">
         <v>8</v>
       </c>
+      <c r="D6">
+        <v>5.369127516778524</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
separate dept from affiliations
</commit_message>
<xml_diff>
--- a/output/2016-10.xlsx
+++ b/output/2016-10.xlsx
@@ -8,14 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="PI hours" sheetId="1" r:id="rId1"/>
-    <sheet name="dept hours" sheetId="2" r:id="rId2"/>
+    <sheet name="department hours" sheetId="2" r:id="rId2"/>
+    <sheet name="unit(accumulative) hours" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
   <si>
     <t>name</t>
   </si>
@@ -29,6 +30,9 @@
     <t>dept</t>
   </si>
   <si>
+    <t>app</t>
+  </si>
+  <si>
     <t>Naira Hovakimyan</t>
   </si>
   <si>
@@ -38,6 +42,15 @@
     <t>Seth Hutchinson</t>
   </si>
   <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>ABE</t>
+  </si>
+  <si>
+    <t>ECE</t>
+  </si>
+  <si>
     <t>['ME', 'AE', 'CSL']</t>
   </si>
   <si>
@@ -47,19 +60,13 @@
     <t>['ECE', 'CSL']</t>
   </si>
   <si>
+    <t>unit(accumulative)</t>
+  </si>
+  <si>
     <t>CSL</t>
   </si>
   <si>
-    <t>ME</t>
-  </si>
-  <si>
     <t>AE</t>
-  </si>
-  <si>
-    <t>ABE</t>
-  </si>
-  <si>
-    <t>ECE</t>
   </si>
 </sst>
 </file>
@@ -417,13 +424,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -436,13 +443,16 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>39</v>
@@ -451,15 +461,18 @@
         <v>70.90909090909091</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>8</v>
@@ -468,15 +481,18 @@
         <v>14.54545454545454</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>8</v>
@@ -485,7 +501,10 @@
         <v>14.54545454545454</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -494,6 +513,72 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>39</v>
+      </c>
+      <c r="D2">
+        <v>70.90909090909091</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>14.54545454545454</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>14.54545454545454</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D6"/>
   <sheetViews>
@@ -503,7 +588,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -517,7 +602,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C2">
         <v>55</v>
@@ -531,7 +616,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>39</v>
@@ -545,7 +630,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C4">
         <v>39</v>
@@ -559,7 +644,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C5">
         <v>8</v>
@@ -573,7 +658,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <v>8</v>

</xml_diff>

<commit_message>
first version adding cfop, working, please revisit
</commit_message>
<xml_diff>
--- a/output/2016-10.xlsx
+++ b/output/2016-10.xlsx
@@ -10,13 +10,14 @@
     <sheet name="PI hours" sheetId="1" r:id="rId1"/>
     <sheet name="department hours" sheetId="2" r:id="rId2"/>
     <sheet name="unit(accumulative) hours" sheetId="3" r:id="rId3"/>
+    <sheet name="cfop hours" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
   <si>
     <t>name</t>
   </si>
@@ -33,6 +34,9 @@
     <t>app</t>
   </si>
   <si>
+    <t>cfop</t>
+  </si>
+  <si>
     <t>Naira Hovakimyan</t>
   </si>
   <si>
@@ -60,6 +64,15 @@
     <t>['ECE', 'CSL']</t>
   </si>
   <si>
+    <t>['cfop_NH']</t>
+  </si>
+  <si>
+    <t>['cfop_GC']</t>
+  </si>
+  <si>
+    <t>['cfop_HUTCHINSON']</t>
+  </si>
+  <si>
     <t>unit(accumulative)</t>
   </si>
   <si>
@@ -67,6 +80,15 @@
   </si>
   <si>
     <t>AE</t>
+  </si>
+  <si>
+    <t>cfop_NH</t>
+  </si>
+  <si>
+    <t>cfop_GC</t>
+  </si>
+  <si>
+    <t>cfop_HUTCHINSON</t>
   </si>
 </sst>
 </file>
@@ -424,13 +446,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -446,13 +468,16 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2">
         <v>39</v>
@@ -461,18 +486,21 @@
         <v>70.90909090909091</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <v>8</v>
@@ -481,18 +509,21 @@
         <v>14.54545454545454</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4">
         <v>8</v>
@@ -501,10 +532,13 @@
         <v>14.54545454545454</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -536,7 +570,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>39</v>
@@ -550,7 +584,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>8</v>
@@ -564,7 +598,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <v>8</v>
@@ -588,7 +622,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -602,7 +636,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C2">
         <v>55</v>
@@ -616,7 +650,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3">
         <v>39</v>
@@ -630,7 +664,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C4">
         <v>39</v>
@@ -644,7 +678,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <v>8</v>
@@ -658,13 +692,79 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6">
         <v>8</v>
       </c>
       <c r="D6">
         <v>5.369127516778524</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2">
+        <v>39</v>
+      </c>
+      <c r="D2">
+        <v>54.92957746478874</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3">
+        <v>16</v>
+      </c>
+      <c r="D3">
+        <v>22.53521126760563</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4">
+        <v>16</v>
+      </c>
+      <c r="D4">
+        <v>22.53521126760563</v>
       </c>
     </row>
   </sheetData>

</xml_diff>